<commit_message>
Rajout répertoire lib dans css et js pour distinguer nos dev des librairies
</commit_message>
<xml_diff>
--- a/Map_site.xlsx
+++ b/Map_site.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>js/fonctionData.js</t>
   </si>
@@ -593,6 +593,23 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">page/parcours_liste.php
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>click bouton liste parcours :
+tableau de tous les parcours</t>
     </r>
   </si>
 </sst>
@@ -957,7 +974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -965,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,41 +1068,46 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="D12" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
@@ -1093,18 +1115,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -1112,43 +1125,57 @@
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
-        <v>5</v>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
formulaire saisie commentaire et note sur un parcours
</commit_message>
<xml_diff>
--- a/Map_site.xlsx
+++ b/Map_site.xlsx
@@ -1616,9 +1616,6 @@
     <t>bouton visualisation_3D.php</t>
   </si>
   <si>
-    <t>page/services proposés php</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1655,9 +1652,6 @@
     </r>
   </si>
   <si>
-    <t>Membre : Saisi Notation et commentaire des parcours effectués</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">fonction/recup_data_commentaire.php
 </t>
@@ -1672,6 +1666,63 @@
       <t>Au chargement du document :
 chargement via ajax des commentaires et notes associés au parcours</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fonction/verif_data_commentaire.php
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Click bouton </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saisir commentaire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supprimer commentaire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :
+ajoute ou supprime un commentaire (et note) du membre connecté  (de type cavalier) pour ce parcours  </t>
+    </r>
+  </si>
+  <si>
+    <t>page/services proposés par un centre équestr</t>
   </si>
 </sst>
 </file>
@@ -1857,7 +1908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1939,6 +1990,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2239,7 +2296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2247,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,10 +2325,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="12" t="s">
@@ -2283,8 +2340,8 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="20"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
@@ -2292,8 +2349,8 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
         <v>59</v>
@@ -2301,8 +2358,8 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
         <v>60</v>
@@ -2310,8 +2367,8 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
         <v>61</v>
@@ -2327,8 +2384,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
         <v>63</v>
@@ -2344,8 +2401,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="10" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="1"/>
       <c r="D7" s="9" t="s">
         <v>64</v>
@@ -2359,8 +2416,8 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="1"/>
       <c r="D8" s="4" t="s">
         <v>65</v>
@@ -2372,8 +2429,8 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" s="10" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="1"/>
       <c r="D9" s="11" t="s">
         <v>66</v>
@@ -2385,8 +2442,8 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:8" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="1"/>
       <c r="D10" s="24" t="s">
         <v>67</v>
@@ -2400,8 +2457,8 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="1"/>
       <c r="D11" s="9"/>
       <c r="E11" s="21" t="s">
@@ -2413,8 +2470,8 @@
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
       <c r="E12" s="7" t="s">
@@ -2429,8 +2486,8 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="1"/>
       <c r="D13" s="4"/>
       <c r="E13" s="7" t="s">
@@ -2447,8 +2504,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4"/>
       <c r="E14" s="7" t="s">
@@ -2465,8 +2522,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="1"/>
       <c r="D15" s="16"/>
       <c r="E15" s="7"/>
@@ -2474,20 +2531,18 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="35"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="18" t="s">
-        <v>74</v>
-      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="1"/>
       <c r="D17" s="18" t="s">
         <v>32</v>
@@ -2497,7 +2552,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="15"/>
       <c r="C18" s="1"/>
       <c r="D18" s="8"/>
@@ -2506,8 +2561,8 @@
       <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="36" t="s">
+      <c r="A19" s="42"/>
+      <c r="B19" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -2516,179 +2571,199 @@
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="37"/>
+      <c r="E20" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="4"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="33" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="37"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="33" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="32"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="5" t="s">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" s="35" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D25" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="1"/>
-      <c r="E24" s="4" t="s">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="1"/>
+      <c r="E26" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="5" t="s">
+    <row r="27" spans="1:7" ht="41.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="38"/>
-      <c r="D26" s="27" t="s">
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="40"/>
+      <c r="D28" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="38"/>
-      <c r="D27" s="27" t="s">
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="40"/>
+      <c r="D29" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="38"/>
-      <c r="D28" s="27" t="s">
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="40"/>
+      <c r="D30" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="38"/>
-      <c r="D29" s="27" t="s">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
+      <c r="B31" s="40"/>
+      <c r="D31" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="38"/>
-      <c r="D30" s="27" t="s">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="42"/>
+      <c r="B32" s="40"/>
+      <c r="D32" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="14"/>
-      <c r="D31" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="22"/>
-      <c r="D32" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-    </row>
-    <row r="33" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="42"/>
       <c r="B33" s="14"/>
       <c r="D33" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-    </row>
-    <row r="34" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="30"/>
-      <c r="D34" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="42"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" spans="1:6" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
-      <c r="B35" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>42</v>
-      </c>
+    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="42"/>
+      <c r="B35" s="14"/>
       <c r="D35" s="18" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
     </row>
-    <row r="38" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="6"/>
+    <row r="36" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42"/>
+      <c r="B36" s="30"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+    </row>
+    <row r="37" spans="1:6" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A37" s="42"/>
+      <c r="B37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+    </row>
+    <row r="40" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:B17"/>
-    <mergeCell ref="B19:B30"/>
-    <mergeCell ref="A1:A35"/>
+    <mergeCell ref="B19:B32"/>
+    <mergeCell ref="A1:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>